<commit_message>
Bugfix return full rowValue instead of substring
</commit_message>
<xml_diff>
--- a/demofiles/books.xlsx
+++ b/demofiles/books.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>book&gt;author&gt;firstName</t>
   </si>
@@ -53,106 +53,156 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Muste</t>
-  </si>
-  <si>
-    <t>Midni</t>
-  </si>
-  <si>
-    <t>Fanta</t>
-  </si>
-  <si>
-    <t>2000-</t>
-  </si>
-  <si>
-    <t>A for</t>
-  </si>
-  <si>
-    <t>Maeve</t>
-  </si>
-  <si>
-    <t>After</t>
-  </si>
-  <si>
-    <t>Coret</t>
-  </si>
-  <si>
-    <t>Obero</t>
-  </si>
-  <si>
-    <t>2001-</t>
-  </si>
-  <si>
-    <t>In po</t>
-  </si>
-  <si>
-    <t>The S</t>
-  </si>
-  <si>
-    <t>The t</t>
-  </si>
-  <si>
-    <t>Lover</t>
-  </si>
-  <si>
-    <t>Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When </t>
-  </si>
-  <si>
-    <t>Randa</t>
-  </si>
-  <si>
-    <t>Splis</t>
-  </si>
-  <si>
-    <t>A dee</t>
-  </si>
-  <si>
-    <t>Thurm</t>
-  </si>
-  <si>
-    <t>Creep</t>
-  </si>
-  <si>
-    <t>Horro</t>
-  </si>
-  <si>
-    <t>An an</t>
-  </si>
-  <si>
-    <t>Knorr</t>
-  </si>
-  <si>
-    <t>Parad</t>
-  </si>
-  <si>
-    <t>Scien</t>
-  </si>
-  <si>
-    <t>Kress</t>
-  </si>
-  <si>
-    <t>Micro</t>
-  </si>
-  <si>
-    <t>Compu</t>
-  </si>
-  <si>
-    <t>O'Bri</t>
-  </si>
-  <si>
-    <t>MSXML</t>
-  </si>
-  <si>
-    <t>The M</t>
-  </si>
-  <si>
-    <t>Visua</t>
-  </si>
-  <si>
-    <t>Galos</t>
+    <t>Mustermann</t>
+  </si>
+  <si>
+    <t>Midnight Rain</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>2000-12-16</t>
+  </si>
+  <si>
+    <t>A former architect battles corporate zombies, 
+      an evil sorceress, and her own childhood to become queen 
+      of the world.</t>
+  </si>
+  <si>
+    <t>Maeve Ascendant</t>
+  </si>
+  <si>
+    <t>2000-11-17</t>
+  </si>
+  <si>
+    <t>After the collapse of a nanotechnology 
+      society in England, the young survivors lay the 
+      foundation for a new society.</t>
+  </si>
+  <si>
+    <t>Corets, Eva</t>
+  </si>
+  <si>
+    <t>Oberon's Legacy</t>
+  </si>
+  <si>
+    <t>2001-03-10</t>
+  </si>
+  <si>
+    <t>In post-apocalypse England, the mysterious 
+      agent known only as Oberon helps to create a new life 
+      for the inhabitants of London. Sequel to Maeve 
+      Ascendant.</t>
+  </si>
+  <si>
+    <t>The Sundered Grail</t>
+  </si>
+  <si>
+    <t>The two daughters of Maeve, half-sisters, 
+      battle one another for control of England. Sequel to 
+      Oberon's Legacy.</t>
+  </si>
+  <si>
+    <t>Lover Birds</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>2000-09-02</t>
+  </si>
+  <si>
+    <t>When Carla meets Paul at an ornithology 
+      conference, tempers fly as feathers get ruffled.</t>
+  </si>
+  <si>
+    <t>Randall, Cynthia</t>
+  </si>
+  <si>
+    <t>Splish Splash</t>
+  </si>
+  <si>
+    <t>2000-11-02</t>
+  </si>
+  <si>
+    <t>A deep sea diver finds true love twenty 
+      thousand leagues beneath the sea.</t>
+  </si>
+  <si>
+    <t>Thurman, Paula</t>
+  </si>
+  <si>
+    <t>Creepy Crawlies</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>2000-12-06</t>
+  </si>
+  <si>
+    <t>An anthology of horror stories about roaches,
+      centipedes, scorpions  and other insects.</t>
+  </si>
+  <si>
+    <t>Knorr, Stefan</t>
+  </si>
+  <si>
+    <t>Paradox Lost</t>
+  </si>
+  <si>
+    <t>Science Fiction</t>
+  </si>
+  <si>
+    <t>After an inadvertant trip through a Heisenberg
+      Uncertainty Device, James Salway discovers the problems 
+      of being quantum.</t>
+  </si>
+  <si>
+    <t>Kress, Peter</t>
+  </si>
+  <si>
+    <t>Microsoft .NET: The Programming Bible</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>2000-12-09</t>
+  </si>
+  <si>
+    <t>Microsoft's .NET initiative is explored in 
+      detail in this deep programmer's reference.</t>
+  </si>
+  <si>
+    <t>O'Brien, Tim</t>
+  </si>
+  <si>
+    <t>MSXML3: A Comprehensive Guide</t>
+  </si>
+  <si>
+    <t>2000-12-01</t>
+  </si>
+  <si>
+    <t>The Microsoft MSXML3 parser is covered in 
+      detail, with attention to XML DOM interfaces, XSLT processing, 
+      SAX and more.</t>
+  </si>
+  <si>
+    <t>Visual Studio 7: A Comprehensive Guide</t>
+  </si>
+  <si>
+    <t>2001-04-16</t>
+  </si>
+  <si>
+    <t>Microsoft Visual Studio 7 is explored in depth,
+      looking at how Visual Basic, Visual C++, C#, and ASP+ are 
+      integrated into a comprehensive development 
+      environment.</t>
+  </si>
+  <si>
+    <t>Galos, Mike</t>
   </si>
 </sst>
 </file>
@@ -571,13 +621,13 @@
         <v>5.95</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -587,7 +637,7 @@
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -596,13 +646,13 @@
         <v>5.95</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -612,7 +662,7 @@
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -622,10 +672,10 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <v>20</v>
@@ -641,22 +691,22 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>4.95</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -666,22 +716,22 @@
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>4.95</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -691,22 +741,22 @@
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>4.95</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -716,22 +766,22 @@
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>6.95</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -741,22 +791,22 @@
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>36.95</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -766,22 +816,22 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>36.95</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -791,22 +841,22 @@
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E12">
         <v>49.95</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>

</xml_diff>